<commit_message>
Final Implementation for Lucrari and Contracte. (Contracte without Beneficiari)
</commit_message>
<xml_diff>
--- a/ContabilitatePrimaraPFA/BugsReportAndTestResults.xlsx
+++ b/ContabilitatePrimaraPFA/BugsReportAndTestResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Bug report</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Area where the bug was find</t>
+  </si>
+  <si>
+    <t>changing the tipe of Lucrare: is setting the first from list</t>
   </si>
 </sst>
 </file>
@@ -129,10 +132,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,11 +442,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -457,13 +460,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>